<commit_message>
get the reasonable calibration resutls
</commit_message>
<xml_diff>
--- a/results/new_results/logistic_params.xlsx
+++ b/results/new_results/logistic_params.xlsx
@@ -1,21 +1,36 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10713"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10720"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Volumes/work/Projects/Fleeting_modeling_SAO/results/new_results/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DD2FF5B9-C706-4445-8233-7B6EA1C16AB7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{286A3F28-DD88-124A-BC75-E67147921F68}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-36780" yWindow="500" windowWidth="36780" windowHeight="21100" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0" calcCompleted="0" calcOnSave="0"/>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$D$50</definedName>
+  </definedNames>
+  <calcPr calcId="191029" calcMode="manual" calcCompleted="0" calcOnSave="0"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
@@ -413,10 +428,14 @@
   <dimension ref="A1:D50"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G32" sqref="G32"/>
+      <selection activeCell="H4" sqref="H4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="15.83203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.1640625" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
@@ -1119,6 +1138,7 @@
       </c>
     </row>
   </sheetData>
+  <autoFilter ref="A1:D50" xr:uid="{00000000-0001-0000-0000-000000000000}"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
</xml_diff>